<commit_message>
Completed the first iteration of changes to support the time zone per Kronos Org Job to Teams mapping.
</commit_message>
<xml_diff>
--- a/Kronos-Shifts-Connector/Excel Templates/KronosShiftTeamDeptMappingTemplate.xlsx
+++ b/Kronos-Shifts-Connector/Excel Templates/KronosShiftTeamDeptMappingTemplate.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-abt\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\OSTeamsConnector\Kronos-Shifts-Connector\Excel Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C3B16C-B502-44E2-9A6F-E4AC26375C47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96E42EF9-69B1-482F-9FB9-1666A2B4B3DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamsDepartmentMappingTemplate" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TeamsDepartmentMappingTemplate!$B$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">TeamsDepartmentMappingTemplate!$A$1:$C$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>KronosOrgJobPath</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>ShiftSchedulingGroupName</t>
+  </si>
+  <si>
+    <t>KronosTimeZone</t>
   </si>
 </sst>
 </file>
@@ -119,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -127,6 +130,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -145,8 +151,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table11" displayName="Table11" ref="C1:F5" totalsRowShown="0">
-  <autoFilter ref="C1:F5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table11" displayName="Table11" ref="D1:G5" totalsRowShown="0">
+  <autoFilter ref="D1:G5" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ShiftTeamId"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="ShiftTeamName"/>
@@ -442,65 +448,70 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="29.3984375" customWidth="1"/>
+    <col min="4" max="4" width="23.3984375" customWidth="1"/>
+    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="C2" s="6"/>
+      <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="7"/>
+      <c r="E3" s="4"/>
+      <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.45">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="C4" s="6"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="7"/>
+      <c r="G5" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1" xr:uid="{3D3912FF-8650-4EDC-B73F-91D41547DA57}"/>
+  <autoFilter ref="A1:C1" xr:uid="{F97C1EB1-9833-4995-9B45-A81ECD27FE2F}"/>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>